<commit_message>
November 9 tomaso evening push 1
</commit_message>
<xml_diff>
--- a/pvr.xlsx
+++ b/pvr.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomasodeponti/Desktop/C&amp;S/Q1/Operations optimisation/project/gurobi trial/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomasodeponti/Desktop/C&amp;S/Q1/Operations optimisation/project/gurobi trial/AE4441-Group-2-VRP-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD03A5B-F1E9-2F48-831E-F9C05438DB47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE856739-F5F0-864F-A147-BD65D31211DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{39CBE691-1030-2142-BE32-D6F89826DDB0}"/>
   </bookViews>
@@ -494,7 +494,7 @@
   <dimension ref="A1:C91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,7 +518,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -531,7 +531,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -544,7 +544,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -570,7 +570,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -583,7 +583,7 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -596,7 +596,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -609,7 +609,7 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -622,7 +622,7 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -635,7 +635,7 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -648,7 +648,7 @@
         <v>3</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -661,7 +661,7 @@
         <v>4</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -674,7 +674,7 @@
         <v>5</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -700,7 +700,7 @@
         <v>7</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -713,7 +713,7 @@
         <v>8</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -726,7 +726,7 @@
         <v>9</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -739,7 +739,7 @@
         <v>10</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -752,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -765,7 +765,7 @@
         <v>2</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -778,7 +778,7 @@
         <v>4</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -791,7 +791,7 @@
         <v>5</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -804,7 +804,7 @@
         <v>6</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -817,7 +817,7 @@
         <v>7</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -830,7 +830,7 @@
         <v>8</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -843,7 +843,7 @@
         <v>9</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -856,7 +856,7 @@
         <v>10</v>
       </c>
       <c r="C28">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -869,7 +869,7 @@
         <v>1</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -882,7 +882,7 @@
         <v>2</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -895,7 +895,7 @@
         <v>3</v>
       </c>
       <c r="C31">
-        <v>5</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -908,7 +908,7 @@
         <v>5</v>
       </c>
       <c r="C32">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -921,7 +921,7 @@
         <v>6</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -934,7 +934,7 @@
         <v>7</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -947,7 +947,7 @@
         <v>8</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -960,7 +960,7 @@
         <v>9</v>
       </c>
       <c r="C36">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -973,7 +973,7 @@
         <v>10</v>
       </c>
       <c r="C37">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -986,7 +986,7 @@
         <v>1</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -999,7 +999,7 @@
         <v>2</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1012,7 +1012,7 @@
         <v>3</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1025,7 +1025,7 @@
         <v>4</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1038,7 +1038,7 @@
         <v>6</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1051,7 +1051,7 @@
         <v>7</v>
       </c>
       <c r="C43">
-        <v>5</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1064,7 +1064,7 @@
         <v>8</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1077,7 +1077,7 @@
         <v>9</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1090,7 +1090,7 @@
         <v>10</v>
       </c>
       <c r="C46">
-        <v>4</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1103,7 +1103,7 @@
         <v>1</v>
       </c>
       <c r="C47">
-        <v>3</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1116,7 +1116,7 @@
         <v>2</v>
       </c>
       <c r="C48">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1129,7 +1129,7 @@
         <v>3</v>
       </c>
       <c r="C49">
-        <v>2</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1142,7 +1142,7 @@
         <v>4</v>
       </c>
       <c r="C50">
-        <v>4</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1155,7 +1155,7 @@
         <v>5</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1168,7 +1168,7 @@
         <v>7</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1181,7 +1181,7 @@
         <v>8</v>
       </c>
       <c r="C53">
-        <v>4</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1194,7 +1194,7 @@
         <v>9</v>
       </c>
       <c r="C54">
-        <v>4</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1207,7 +1207,7 @@
         <v>10</v>
       </c>
       <c r="C55">
-        <v>5</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1220,7 +1220,7 @@
         <v>1</v>
       </c>
       <c r="C56">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1233,7 +1233,7 @@
         <v>2</v>
       </c>
       <c r="C57">
-        <v>4</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1246,7 +1246,7 @@
         <v>3</v>
       </c>
       <c r="C58">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -1259,7 +1259,7 @@
         <v>4</v>
       </c>
       <c r="C59">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -1272,7 +1272,7 @@
         <v>5</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -1285,7 +1285,7 @@
         <v>6</v>
       </c>
       <c r="C61">
-        <v>2</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -1298,7 +1298,7 @@
         <v>8</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -1311,7 +1311,7 @@
         <v>9</v>
       </c>
       <c r="C63">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -1324,7 +1324,7 @@
         <v>10</v>
       </c>
       <c r="C64">
-        <v>4</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -1337,7 +1337,7 @@
         <v>1</v>
       </c>
       <c r="C65">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -1350,7 +1350,7 @@
         <v>2</v>
       </c>
       <c r="C66">
-        <v>2</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -1363,7 +1363,7 @@
         <v>3</v>
       </c>
       <c r="C67">
-        <v>5</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -1376,7 +1376,7 @@
         <v>4</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>88</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -1389,7 +1389,7 @@
         <v>5</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -1402,7 +1402,7 @@
         <v>6</v>
       </c>
       <c r="C70">
-        <v>4</v>
+        <v>91</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -1415,7 +1415,7 @@
         <v>7</v>
       </c>
       <c r="C71">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -1428,7 +1428,7 @@
         <v>9</v>
       </c>
       <c r="C72">
-        <v>5</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -1441,7 +1441,7 @@
         <v>10</v>
       </c>
       <c r="C73">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -1454,7 +1454,7 @@
         <v>1</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>79</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -1467,7 +1467,7 @@
         <v>2</v>
       </c>
       <c r="C75">
-        <v>3</v>
+        <v>86</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -1480,7 +1480,7 @@
         <v>3</v>
       </c>
       <c r="C76">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -1493,7 +1493,7 @@
         <v>4</v>
       </c>
       <c r="C77">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -1506,7 +1506,7 @@
         <v>5</v>
       </c>
       <c r="C78">
-        <v>4</v>
+        <v>58</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -1519,7 +1519,7 @@
         <v>6</v>
       </c>
       <c r="C79">
-        <v>3</v>
+        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -1532,7 +1532,7 @@
         <v>7</v>
       </c>
       <c r="C80">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -1545,7 +1545,7 @@
         <v>8</v>
       </c>
       <c r="C81">
-        <v>4</v>
+        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -1558,7 +1558,7 @@
         <v>10</v>
       </c>
       <c r="C82">
-        <v>5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -1571,7 +1571,7 @@
         <v>1</v>
       </c>
       <c r="C83">
-        <v>4</v>
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -1584,7 +1584,7 @@
         <v>2</v>
       </c>
       <c r="C84">
-        <v>3</v>
+        <v>96</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -1597,7 +1597,7 @@
         <v>3</v>
       </c>
       <c r="C85">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -1610,7 +1610,7 @@
         <v>4</v>
       </c>
       <c r="C86">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -1623,7 +1623,7 @@
         <v>5</v>
       </c>
       <c r="C87">
-        <v>3</v>
+        <v>79</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -1636,7 +1636,7 @@
         <v>6</v>
       </c>
       <c r="C88">
-        <v>2</v>
+        <v>67</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -1649,7 +1649,7 @@
         <v>7</v>
       </c>
       <c r="C89">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -1662,7 +1662,7 @@
         <v>8</v>
       </c>
       <c r="C90">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -1675,7 +1675,7 @@
         <v>9</v>
       </c>
       <c r="C91">
-        <v>5</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>